<commit_message>
making a lot of changes, adding instructions
</commit_message>
<xml_diff>
--- a/demo_data/1min.xlsx
+++ b/demo_data/1min.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/DuyNguyen/Projects/bioretention_mechanisms_2.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/DuyNguyen/Projects/bioretention_rain/demo_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_3FE2423402D1121E52FF31D2F8375B06049B3EE4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F47B698-6731-4AC5-9008-7F9EAE262CAF}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_3FE2423402D1121E52FF31D2F8375B06049B3EE4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EC830D5-CFBC-49A6-9454-F7B2D2D67717}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="rainfall_data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -25,7 +25,7 @@
     <t>datetime</t>
   </si>
   <si>
-    <t>r3ba1r01r</t>
+    <t>rainfall_value</t>
   </si>
 </sst>
 </file>
@@ -434,13 +434,13 @@
   <dimension ref="A1:B9350"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -75518,9 +75518,29 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CFE3202-C0B6-4EB0-B1CE-12D39E4D9208}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CFE3202-C0B6-4EB0-B1CE-12D39E4D9208}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="02ea596c-bf3f-4512-ad68-024a720c79b2"/>
+    <ds:schemaRef ds:uri="959569b2-1f16-4dd0-b5ed-bb064e5cd07e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF230723-0E5A-4424-91D6-3445189C35A7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF230723-0E5A-4424-91D6-3445189C35A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
The rainfall and flow are done. Need to QA, fix little details
</commit_message>
<xml_diff>
--- a/demo_data/1min.xlsx
+++ b/demo_data/1min.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/DuyNguyen/Projects/bioretention_rain/demo_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_3FE2423402D1121E52FF31D2F8375B06049B3EE4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EC830D5-CFBC-49A6-9454-F7B2D2D67717}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_3FE2423402D1121E52FF31D2F8375B06049B3EE4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DEE7440-A2FD-470D-9024-9EA4F5DBADC4}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rainfall_data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <t>datetime</t>
   </si>
   <si>
-    <t>rainfall_value</t>
+    <t>rain</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A1:B9350"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
put instructions in the downloaded files
</commit_message>
<xml_diff>
--- a/demo_data/1min.xlsx
+++ b/demo_data/1min.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/DuyNguyen/Projects/bioretention_rain/demo_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/DuyNguyen/Projects/rainfall_flow_calculator_shiny/demo_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_7BC79D5E344B00FC4EC4AEBD32F929AA8D3C4DD2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B706D6C9-734B-49B1-9026-EF798DB2EB3A}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_7BC79D5E344B00FC4EC4AEBD32F929AA8D3C4DD2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F201E8EB-ED6F-47F0-A763-4FD159915E84}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="165" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="2" r:id="rId1"/>
+    <sheet name="rain_data" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -93,6 +94,333 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B79A098B-6CAD-4FCF-8E22-1BBA1049B1B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="19050"/>
+          <a:ext cx="8229599" cy="9772650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Application Usage Guide</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>=======================</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>This guide provides instructions for using the application and outlines the data requirements for successful analysis.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Analysis Types</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>--------------</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>IMPORTANT: The column names and tab names in the templates (both rainfall and flow) must remain unchanged for accurate analysis and app's functionality.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>The application supports two types of analysis: Rainfall Analysis and Flow Analysis. In the zip package that </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Rainfall Analysis</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>-----------------</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>To perform a Rainfall Analysis, follow these steps:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1. Open the rainfall template (rainfall_template.xlsx).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>2. Copy and paste the rainfall data into the template.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>3. Ensure that the rain gauge values are entered into the designated rain column within the template.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Demo data is available for flow analysis under demo_data folder.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Flow Analysis</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>-------------</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>To perform a Flow Analysis, follow these steps:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1. Open the flow template (flow_template.xlsx).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>2. Copy and paste the flow data from your datasheet into the downloaded template.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>3. Accommodate up to four flows for analysis: inflow 1, inflow 2, outflow, and bypass.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>4. Refer to the Methods tab in the template for an illustration of the possible flow type configurations.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>5. You are not required to submit data for all four flow types; any combination of flow types is acceptable.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>IMPORTANT: If any of the flow data types are not applicable, leave the corresponding tab blank. Do not modify the columns or the tab names.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Demo data is available for flow analysis under demo_data folder.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Data Requirements</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>-----------------</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>To ensure successful analysis, the uploaded Excel spreadsheet must conform to the following requirements:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>- Flow must be reported in units of L/s, gpm, or cfs.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>- The timestamp should be in 24-hour format (mm/dd/yy hh:mm:ss).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>- Each tab must contain exactly two columns: one for the sample timestamps data and one for the associated values.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>- The column names and the tab names must not be changed from the template.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Please ensure that your data meets these requirements before using the application for analysis.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>For further assistance or inquiries, please contact our support team at stormwater@sccwrp.org</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -415,6 +743,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72295B29-DEB2-4219-BF6E-4F2B4C7327AC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9350"/>
   <sheetViews>
@@ -75231,15 +75574,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21cacd0d90dbd8beb6fc12ad84d4cd0e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b418c8325abc32123734ac979891270" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -75499,15 +75833,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59CA2C8-7811-4302-B3FE-FC4240DB0682}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{540529D9-4031-4576-9897-CF10F33AAF2D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -75525,4 +75860,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59CA2C8-7811-4302-B3FE-FC4240DB0682}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed a few minor things
</commit_message>
<xml_diff>
--- a/demo_data/1min.xlsx
+++ b/demo_data/1min.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/DuyNguyen/Projects/rainfall_flow_calculator_shiny/demo_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_7BC79D5E344B00FC4EC4AEBD32F929AA8D3C4DD2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F201E8EB-ED6F-47F0-A763-4FD159915E84}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_7BC79D5E344B00FC4EC4AEBD32F929AA8D3C4DD2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01858720-5582-481D-8C3D-6FFDCE74C2E7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -160,261 +160,467 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>Application Usage Guide</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>=======================</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>This guide provides instructions for using the application and outlines the data requirements for successful analysis.</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>Analysis Types</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>--------------</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>IMPORTANT: The column names and tab names in the templates (both rainfall and flow) must remain unchanged for accurate analysis and app's functionality.</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>The application supports two types of analysis: Rainfall Analysis and Flow Analysis. In the zip package that </a:t>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The application supports two types of analysis: Rainfall Analysis and Flow Analysis. </a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Rainfall Analysis</a:t>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>---------------------</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>-----------------</a:t>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Rainfall Analysis</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: The user is advised to copy and paste the rainfall data, whether it is in the form of 1-minute or time-of-tips data, into the downloaded template. It is important to note that the rain gauge values must be entered into the designated rain column within the template. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>A user can submit a continuous rainfall record without skipping any timestamps, containing multiple events in a single file.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>To perform a Rainfall Analysis, follow these steps:</a:t>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Demo data are available on the Shin</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>y App.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>1. Open the rainfall template (rainfall_template.xlsx).</a:t>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>---------------------</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>2. Copy and paste the rainfall data into the template.</a:t>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Flow</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> Analysis</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Flow data should be copy-pasted from the user's datasheet to the downloaded data template. Up to four flows can be accomodated for analysis. The available flow types are inflow 1, inflow 2, outflow and bypass. Refer to the Methods tab for an illustration of the possible flow type configurations. A user does not need to submit all four types, any combination of the flow types is acceptable. A user can only submit flow data for a single rain event. If any of the data types are not applicable, leave the tab blank (as is)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Demo data are available on the Shin</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>y App.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>3. Ensure that the rain gauge values are entered into the designated rain column within the template.</a:t>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>---------------------</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Demo data is available for flow analysis under demo_data folder.</a:t>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Data Requirements</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Flow Analysis</a:t>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>---------------------</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>-------------</a:t>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>To ensure successful analysis, the uploaded Excel spreadsheet must conform to the following requirements:</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>To perform a Flow Analysis, follow these steps:</a:t>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- Flow must be reported in units of L/s, gpm, or cfs.</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>1. Open the flow template (flow_template.xlsx).</a:t>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- The timestamp should be in 24-hour format (mm/dd/yy hh:mm:ss).</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>2. Copy and paste the flow data from your datasheet into the downloaded template.</a:t>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- Each tab must contain exactly two columns: one for the sample timestamps data and one for the associated values.</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>3. Accommodate up to four flows for analysis: inflow 1, inflow 2, outflow, and bypass.</a:t>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- The column names and the tab names must not be changed from the template.</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>4. Refer to the Methods tab in the template for an illustration of the possible flow type configurations.</a:t>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Please ensure that your data meets these requirements before using the application for analysis.</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>5. You are not required to submit data for all four flow types; any combination of flow types is acceptable.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>IMPORTANT: If any of the flow data types are not applicable, leave the corresponding tab blank. Do not modify the columns or the tab names.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Demo data is available for flow analysis under demo_data folder.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Data Requirements</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>-----------------</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>To ensure successful analysis, the uploaded Excel spreadsheet must conform to the following requirements:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>- Flow must be reported in units of L/s, gpm, or cfs.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>- The timestamp should be in 24-hour format (mm/dd/yy hh:mm:ss).</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>- Each tab must contain exactly two columns: one for the sample timestamps data and one for the associated values.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>- The column names and the tab names must not be changed from the template.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Please ensure that your data meets these requirements before using the application for analysis.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>For further assistance or inquiries, please contact our support team at stormwater@sccwrp.org</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -424,9 +630,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -464,9 +670,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -499,26 +705,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -551,26 +740,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -746,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72295B29-DEB2-4219-BF6E-4F2B4C7327AC}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,7 +933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9350"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -75574,8 +75746,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21cacd0d90dbd8beb6fc12ad84d4cd0e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b418c8325abc32123734ac979891270" ns1:_="" ns2:_="" ns3:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02ea596c-bf3f-4512-ad68-024a720c79b2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="582b150a9eb9a8984bd6398cf909f49d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a4808acce3a6e68b39fbd804e31fb38" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="02ea596c-bf3f-4512-ad68-024a720c79b2"/>
     <xsd:import namespace="959569b2-1f16-4dd0-b5ed-bb064e5cd07e"/>
@@ -75602,6 +75796,7 @@
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -75690,6 +75885,11 @@
     <xsd:element name="MediaServiceSearchProperties" ma:index="25" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="26" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -75833,17 +76033,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59CA2C8-7811-4302-B3FE-FC4240DB0682}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{540529D9-4031-4576-9897-CF10F33AAF2D}">
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91475E90-BE31-4491-A407-D9A4D3F0DE0C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="02ea596c-bf3f-4512-ad68-024a720c79b2"/>
+    <ds:schemaRef ds:uri="959569b2-1f16-4dd0-b5ed-bb064e5cd07e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17435B8E-D2C7-4800-AE21-F9A503F5BA31}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -75860,12 +76071,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59CA2C8-7811-4302-B3FE-FC4240DB0682}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>